<commit_message>
commit ob and to
</commit_message>
<xml_diff>
--- a/OfficialBusinessExport.xlsx
+++ b/OfficialBusinessExport.xlsx
@@ -96,7 +96,7 @@
     <t>No.</t>
   </si>
   <si>
-    <t>2020-006</t>
+    <t>2020-007</t>
   </si>
   <si>
     <t>Date:</t>
@@ -117,25 +117,25 @@
     <t>purpose (s).</t>
   </si>
   <si>
-    <t>Test for system</t>
+    <t>RO</t>
   </si>
   <si>
     <t>Place to be visited:</t>
   </si>
   <si>
-    <t>Regional Office</t>
-  </si>
-  <si>
     <t xml:space="preserve">Time of Departure: </t>
   </si>
   <si>
     <t>07:00:00</t>
   </si>
   <si>
+    <t>May 01, 2020</t>
+  </si>
+  <si>
     <t>Time of Return:</t>
   </si>
   <si>
-    <t>17:00:00</t>
+    <t>18:00:00</t>
   </si>
   <si>
     <t>Signature of Requesting Employee (s)</t>
@@ -279,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -340,29 +340,32 @@
     <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,7 +855,7 @@
   <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -863,7 +866,7 @@
     <col min="5" max="5" width="10.42578125" customWidth="true" style="0"/>
     <col min="6" max="6" width="13.28515625" customWidth="true" style="0"/>
     <col min="7" max="7" width="12.140625" customWidth="true" style="0"/>
-    <col min="8" max="8" width="8" customWidth="true" style="0"/>
+    <col min="8" max="8" width="3.140625" customWidth="true" style="0"/>
     <col min="11" max="11" width="9.140625" customWidth="true" style="0"/>
     <col min="12" max="12" width="13.42578125" customWidth="true" style="0"/>
   </cols>
@@ -913,29 +916,29 @@
       <c r="I12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="24"/>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:12">
       <c r="I13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="23"/>
+      <c r="K13" s="24"/>
     </row>
     <row r="16" spans="1:12" customHeight="1" ht="15.75">
       <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
       <c r="I16" s="2" t="s">
         <v>14</v>
       </c>
@@ -944,50 +947,50 @@
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
     </row>
     <row r="19" spans="1:12" customHeight="1" ht="15.75">
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
+      <c r="D19" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
       <c r="H19" s="4"/>
       <c r="I19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="K19" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="23"/>
+      <c r="L19" s="24"/>
     </row>
     <row r="21" spans="1:12" customHeight="1" ht="15.75">
       <c r="B21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
+      <c r="D21" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
       <c r="I21" t="s">
         <v>21</v>
       </c>
-      <c r="K21" s="23" t="s">
+      <c r="K21" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="L21" s="23"/>
+      <c r="L21" s="24"/>
     </row>
     <row r="24" spans="1:12">
       <c r="I24" t="s">
@@ -995,12 +998,12 @@
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="I26" s="23" t="s">
+      <c r="I26" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
     </row>
     <row r="27" spans="1:12">
       <c r="B27" s="5" t="s">
@@ -1014,11 +1017,11 @@
     </row>
     <row r="30" spans="1:12">
       <c r="B30" s="17"/>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D30" s="17"/>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="22" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1122,10 +1125,10 @@
       <c r="I50" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J50" s="20" t="s">
+      <c r="J50" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K50" s="20"/>
+      <c r="K50" s="26"/>
       <c r="L50" s="8"/>
     </row>
     <row r="51" spans="1:12">
@@ -1139,10 +1142,10 @@
       <c r="I51" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J51" s="20" t="s">
+      <c r="J51" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="K51" s="20"/>
+      <c r="K51" s="26"/>
       <c r="L51" s="8"/>
     </row>
     <row r="52" spans="1:12">
@@ -1178,11 +1181,11 @@
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
-      <c r="F54" s="20" t="s">
+      <c r="F54" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="28"/>
       <c r="I54" s="8" t="s">
         <v>14</v>
       </c>
@@ -1194,14 +1197,14 @@
       <c r="B55" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
-      <c r="H55" s="22"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
       <c r="I55" s="8"/>
       <c r="J55" s="8"/>
       <c r="K55" s="8"/>
@@ -1225,21 +1228,21 @@
         <v>17</v>
       </c>
       <c r="C57" s="8"/>
-      <c r="D57" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
+      <c r="D57" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
       <c r="H57" s="12"/>
       <c r="I57" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J57" s="8"/>
+      <c r="K57" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="J57" s="8"/>
-      <c r="K57" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="L57" s="20"/>
+      <c r="L57" s="26"/>
     </row>
     <row r="58" spans="1:12">
       <c r="B58" s="8"/>
@@ -1259,21 +1262,21 @@
         <v>10</v>
       </c>
       <c r="C59" s="8"/>
-      <c r="D59" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
+      <c r="D59" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
       <c r="I59" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J59" s="8"/>
-      <c r="K59" s="20" t="s">
+      <c r="K59" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="L59" s="20"/>
+      <c r="L59" s="26"/>
     </row>
     <row r="60" spans="1:12">
       <c r="B60" s="8"/>
@@ -1337,12 +1340,12 @@
       <c r="F64" s="8"/>
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
-      <c r="I64" s="20" t="s">
+      <c r="I64" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="J64" s="20"/>
-      <c r="K64" s="20"/>
-      <c r="L64" s="20"/>
+      <c r="J64" s="26"/>
+      <c r="K64" s="26"/>
+      <c r="L64" s="26"/>
     </row>
     <row r="65" spans="1:12">
       <c r="B65" s="10" t="s">
@@ -1389,11 +1392,11 @@
     </row>
     <row r="68" spans="1:12">
       <c r="B68" s="18"/>
-      <c r="C68" s="25" t="s">
+      <c r="C68" s="20" t="s">
         <v>26</v>
       </c>
       <c r="D68" s="19"/>
-      <c r="E68" s="25" t="s">
+      <c r="E68" s="20" t="s">
         <v>27</v>
       </c>
       <c r="F68" s="8"/>
@@ -1468,14 +1471,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <sheetProtection password="DD3C" sheet="true" objects="false" scenarios="false" formatCells="true" formatColumns="false" formatRows="false" insertColumns="false" insertRows="true" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="true" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="K59:L59"/>
     <mergeCell ref="I64:L64"/>
     <mergeCell ref="D19:G19"/>
     <mergeCell ref="D57:G57"/>
@@ -1488,6 +1485,12 @@
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="I26:L26"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="K59:L59"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commits ob and to
</commit_message>
<xml_diff>
--- a/OfficialBusinessExport.xlsx
+++ b/OfficialBusinessExport.xlsx
@@ -44,13 +44,13 @@
     <t>No.</t>
   </si>
   <si>
-    <t>2020-007</t>
+    <t>2020-006</t>
   </si>
   <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>May 04, 2020</t>
+    <t>April 30, 2020</t>
   </si>
   <si>
     <t>Permission is requested by Mr./Ms.</t>
@@ -65,25 +65,25 @@
     <t>purpose (s).</t>
   </si>
   <si>
-    <t>RO</t>
+    <t>Test for system</t>
   </si>
   <si>
     <t>Place to be visited:</t>
   </si>
   <si>
+    <t>Regional Office</t>
+  </si>
+  <si>
     <t xml:space="preserve">Time of Departure: </t>
   </si>
   <si>
     <t>07:00:00</t>
   </si>
   <si>
-    <t>May 01, 2020</t>
-  </si>
-  <si>
     <t>Time of Return:</t>
   </si>
   <si>
-    <t>18:00:00</t>
+    <t>17:00:00</t>
   </si>
   <si>
     <t>Signature of Requesting Employee (s)</t>
@@ -1030,18 +1030,18 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="11"/>
       <c r="I19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L19" s="13"/>
     </row>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="13" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -1508,18 +1508,18 @@
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E56" s="14"/>
       <c r="F56" s="14"/>
       <c r="G56" s="14"/>
       <c r="H56" s="11"/>
       <c r="I56" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L56" s="13"/>
     </row>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="13" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>

</xml_diff>